<commit_message>
Upgrade Polars to 1.0.0
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\groupby\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53907EF5-A33E-405A-911F-1A6EF8DCEE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21720" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -41,20 +35,12 @@
     <t>四, Tablet, 五
 六, 七, Vanilla</t>
   </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">afaf
-afaf
-aff </t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,67 +69,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="1">
+    <dxf/>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Frame0" displayName="Frame0" ref="A1:C3" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:C3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="concat" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{F6A8FA8C-1B3F-4602-A528-4F39491A61D9}" name="Column1" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Name" dataDxfId="0"/>
+    <tableColumn id="2" name="concat" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -181,7 +137,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -215,7 +171,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -250,10 +205,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -426,41 +380,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="30.5703125" style="4"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>